<commit_message>
Changed terminal block from 8 to 10 to allow for DUT to have 2 connections. 1 used to connect the DUT, the other used to measure the DUT
</commit_message>
<xml_diff>
--- a/BOM/Bill of Materials-ElectronicLoad.xlsx
+++ b/BOM/Bill of Materials-ElectronicLoad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ART\ElectronicLoad\ElectronicLoad\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66A18492-0113-4FDC-9FC8-5722ACBCC126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C07A0E50-82ED-4479-828A-67D1664D9843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="3765" windowWidth="21600" windowHeight="7245" xr2:uid="{33168AB2-D9A5-4E11-BCAD-2226C4630400}"/>
+    <workbookView xWindow="-24735" yWindow="315" windowWidth="21600" windowHeight="10605" xr2:uid="{EE07FD84-60F7-4F7D-B139-C62F83799CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-ElectronicLoa" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -78,10 +76,10 @@
     <t/>
   </si>
   <si>
-    <t>CONN8</t>
-  </si>
-  <si>
-    <t>Conn Terminal Block 8 POS 2.54mm Solder ST Thru-Hole 6A</t>
+    <t>CONN10_2</t>
+  </si>
+  <si>
+    <t>Conn Terminal Block 10 POS 2.54mm Solder ST Thru-Hole 6A</t>
   </si>
   <si>
     <t>J1</t>
@@ -90,7 +88,7 @@
     <t>On-Shore Technology</t>
   </si>
   <si>
-    <t>OSTVN08A150</t>
+    <t>OSTVN10A150</t>
   </si>
   <si>
     <t>Volume Production</t>
@@ -99,7 +97,7 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>ED10566-ND</t>
+    <t>ED10567-ND</t>
   </si>
   <si>
     <t>MTP3055VL</t>
@@ -230,16 +228,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,261 +545,257 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7456193-960D-4C1A-B9D6-A7EBC1FB40AE}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D25EFD-96A7-48C8-A4BA-F927D359A25E}">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="1" max="1" width="8.5859375" customWidth="1"/>
+    <col min="2" max="2" width="16.234375" customWidth="1"/>
+    <col min="3" max="3" width="12.703125" customWidth="1"/>
+    <col min="4" max="4" width="12.41015625" customWidth="1"/>
+    <col min="5" max="5" width="10.52734375" customWidth="1"/>
+    <col min="6" max="6" width="15.64453125" customWidth="1"/>
+    <col min="7" max="7" width="25.52734375" customWidth="1"/>
+    <col min="8" max="8" width="22.29296875" customWidth="1"/>
+    <col min="9" max="9" width="11.703125" customWidth="1"/>
+    <col min="10" max="10" width="21.52734375" customWidth="1"/>
+    <col min="11" max="11" width="19.3515625" customWidth="1"/>
+    <col min="12" max="12" width="18.5859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="4">
-        <v>2.48</v>
-      </c>
-      <c r="L2" s="4">
-        <v>2.48</v>
+      <c r="K2" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="1">
         <v>1.55</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="1">
         <v>1.55</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="4">
-        <v>1.18</v>
-      </c>
-      <c r="L4" s="4">
-        <v>14.21</v>
+      <c r="K4" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="L4" s="1">
+        <v>15.66</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="1">
         <v>1.55</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="1">
         <v>1.55</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="1">
         <v>0.39</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="1">
         <v>0.39</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="63" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>